<commit_message>
update to data file
</commit_message>
<xml_diff>
--- a/Residue Chain Data Cooker.xlsx
+++ b/Residue Chain Data Cooker.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-19200" yWindow="0" windowWidth="19200" windowHeight="21160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -203,7 +203,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,8 +238,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -270,6 +278,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -280,7 +293,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -289,8 +302,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -435,8 +449,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="8"/>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="8" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
+    <cellStyle name="Bad" xfId="8" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -885,12 +902,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="2072084232"/>
-        <c:axId val="2072048008"/>
+        <c:axId val="2145701608"/>
+        <c:axId val="2145708888"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="2072084232"/>
+        <c:axId val="2145701608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -931,7 +948,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2072048008"/>
+        <c:crossAx val="2145708888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -941,7 +958,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2072048008"/>
+        <c:axId val="2145708888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -988,7 +1005,7 @@
         <c:spPr>
           <a:ln w="12700"/>
         </c:spPr>
-        <c:crossAx val="2072084232"/>
+        <c:crossAx val="2145701608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1432,12 +1449,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-2146294520"/>
-        <c:axId val="-2146288952"/>
+        <c:axId val="2145788760"/>
+        <c:axId val="2145794312"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-2146294520"/>
+        <c:axId val="2145788760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1467,7 +1484,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146288952"/>
+        <c:crossAx val="2145794312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1475,7 +1492,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2146288952"/>
+        <c:axId val="2145794312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1518,7 +1535,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146294520"/>
+        <c:crossAx val="2145788760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2067,12 +2084,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-2140776840"/>
-        <c:axId val="-2140771320"/>
+        <c:axId val="2145829992"/>
+        <c:axId val="2145835496"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-2140776840"/>
+        <c:axId val="2145829992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2102,7 +2119,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140771320"/>
+        <c:crossAx val="2145835496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2111,7 +2128,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2140771320"/>
+        <c:axId val="2145835496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2149,7 +2166,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140776840"/>
+        <c:crossAx val="2145829992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2566,8 +2583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4963,32 +4980,32 @@
       <c r="A44" s="31">
         <v>43</v>
       </c>
-      <c r="B44" s="51" t="s">
+      <c r="B44" s="118" t="s">
         <v>55</v>
       </c>
-      <c r="C44" s="51"/>
-      <c r="D44" s="114">
+      <c r="C44" s="118"/>
+      <c r="D44" s="119">
         <v>112.557</v>
       </c>
-      <c r="E44" s="114">
+      <c r="E44" s="119">
         <v>8.3160000000000007</v>
       </c>
-      <c r="F44" s="114">
+      <c r="F44" s="119">
         <v>65.248999999999995</v>
       </c>
-      <c r="G44" s="114">
+      <c r="G44" s="119">
         <v>67.534999999999997</v>
       </c>
-      <c r="H44" s="114">
+      <c r="H44" s="119">
         <v>60.552999999999997</v>
       </c>
-      <c r="I44" s="114">
+      <c r="I44" s="119">
         <v>70.685000000000002</v>
       </c>
-      <c r="J44" s="114">
+      <c r="J44" s="119">
         <v>60.527000000000001</v>
       </c>
-      <c r="K44" s="114">
+      <c r="K44" s="119">
         <v>70.718999999999994</v>
       </c>
       <c r="L44" s="11">

</xml_diff>